<commit_message>
Allow user to chose the analysis expected to be performed by the BfR
Ticket: SiLeBAT/mibi-portal-client#258
Change-Id: I92d5f4e58e5d9c50aec3d56445fe8e45215746a7
</commit_message>
<xml_diff>
--- a/testData/mps155_timezone_bug_validated.xlsx
+++ b/testData/mps155_timezone_bug_validated.xlsx
@@ -9026,9 +9026,7 @@
       <c r="M14" s="235"/>
       <c r="N14" s="235"/>
       <c r="O14" s="236"/>
-      <c r="P14" t="s" s="137">
-        <v>208</v>
-      </c>
+      <c r="P14" s="137"/>
       <c r="Q14" s="153"/>
       <c r="R14" s="153"/>
       <c r="S14" s="153"/>
@@ -9176,9 +9174,7 @@
       <c r="M19" s="232"/>
       <c r="N19" s="232"/>
       <c r="O19" s="233"/>
-      <c r="P19" t="s" s="137">
-        <v>208</v>
-      </c>
+      <c r="P19" s="137"/>
       <c r="Q19" s="153"/>
       <c r="R19" s="153"/>
       <c r="S19" s="153"/>
@@ -9311,7 +9307,9 @@
       <c r="G24" s="140"/>
       <c r="H24" s="140"/>
       <c r="I24" s="140"/>
-      <c r="J24" s="228"/>
+      <c r="J24" t="s" s="228">
+        <v>208</v>
+      </c>
       <c r="K24" s="229"/>
       <c r="L24" s="229"/>
       <c r="M24" s="229"/>

</xml_diff>

<commit_message>
NRL standard analysis procedures should be marked as 'Standard' in the sample sheet send as PDF to the user.
- Renamed Einsendbogen to SampleSheet
- Moved duplicated code to new SampleSheetService
- Excel/PDF-Services uses SampleSheet instead of SampleSet data structures
- Removed NRLService reference from SampelEntity
- Moved nrl long names to sample-sheet.strings
- Some refactoring and renames here and there

Integration Tests
- Removed invalid ZSP tests for year 2020
- Applied some changes of last few tickets

Ticket: mibi-portal-client#330
Change-Id: Ib879b1bc4e72d6e26b71cf884c56d03c4802d40b
</commit_message>
<xml_diff>
--- a/testData/mps155_timezone_bug_validated.xlsx
+++ b/testData/mps155_timezone_bug_validated.xlsx
@@ -8821,7 +8821,7 @@
         <v>87</v>
       </c>
       <c r="B7" t="s" s="226">
-        <v>76</v>
+        <v>208</v>
       </c>
       <c r="C7" s="226"/>
       <c r="D7" s="226"/>
@@ -9234,7 +9234,9 @@
       <c r="M21" s="232"/>
       <c r="N21" s="232"/>
       <c r="O21" s="233"/>
-      <c r="P21" s="137"/>
+      <c r="P21" t="s" s="137">
+        <v>208</v>
+      </c>
       <c r="Q21" s="153"/>
       <c r="R21" s="153"/>
       <c r="S21" s="153"/>

</xml_diff>